<commit_message>
new version saep readme
</commit_message>
<xml_diff>
--- a/EDA/SAEP_README.xlsx
+++ b/EDA/SAEP_README.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Currently in Service</t>
+          <t>SAEP currently in service</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,12 +486,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Functionality of the SAEP</t>
+          <t>The SAEP has production meters</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The operational status of the SAEP, including the functionality of all critical components such as treatment facilities, distribution networks, and storage systems.</t>
+          <t>The presence of meters that quantify the total water produced by the SAEP.</t>
         </is>
       </c>
     </row>
@@ -501,12 +501,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Is the Water Distributed per Household Sufficient?</t>
+          <t>The SAEP has distribution meters</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>An evaluation of whether the volume of water distributed to each household meets the required minimum standards for daily usage.</t>
+          <t>The presence of meters that measure the volume of water distributed through the network.</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Is It Securely Managed?</t>
+          <t>The SAEP has connection/consumption meters</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>An assessment of the security measures in place to protect the water supply from contamination, theft, and unauthorized access.</t>
+          <t>The availability of meters that record the amount of water consumed by end users.</t>
         </is>
       </c>
     </row>
@@ -531,12 +531,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Is There Production Meters?</t>
+          <t>SAEP Capacity Used</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>The presence of meters that quantify the total water produced by the SAEP.</t>
+          <t>The percentage of the total production capacity of the SAEP that is actually being utilized to serve the population.</t>
         </is>
       </c>
     </row>
@@ -546,12 +546,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Is There Distribution Meters?</t>
+          <t>SAEP Coverage Rate</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The presence of meters that measure the volume of water distributed through the network.</t>
+          <t>The proportion of the target population that has access to the services provided by the SAEP within its operational area.</t>
         </is>
       </c>
     </row>
@@ -561,12 +561,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Is There Consumption Meters?</t>
+          <t># of Employees</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>The availability of meters that record the amount of water consumed by end users.</t>
+          <t>The total number of personnel employed by the SAEP organization.</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Is There Sufficient Water per Household?</t>
+          <t># of Active Subscribers at the Start of the Month</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Similar to 'Is the Water Distributed per Household Sufficient?', this measures if households receive enough water to meet their needs.</t>
+          <t>The number of active subscribers (those receiving and paying for water services) at the beginning of the month.</t>
         </is>
       </c>
     </row>
@@ -591,12 +591,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SAEP Capacity Used</t>
+          <t># of Active Subscribers at the End of the Month</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>The percentage of the total production capacity of the SAEP that is actually being utilized to serve the population.</t>
+          <t>The number of active subscribers at the end of the month.</t>
         </is>
       </c>
     </row>
@@ -606,12 +606,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SAEP Coverage Rate</t>
+          <t># of Passive Subscribers at the End of the Month</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>The proportion of the target population that has access to the services provided by the SAEP within its operational area.</t>
+          <t>The number of subscribers who are registered but are not actively receiving water services at the end of the month.</t>
         </is>
       </c>
     </row>
@@ -621,12 +621,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t># of Employees</t>
+          <t># of Suspended Subscribers at the End of the Month</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The total number of personnel employed by the SAEP organization.</t>
+          <t>The number of subscribers whose services have been temporarily suspended by the end of the month.</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t># of Active Subscribers at the Start of the Month</t>
+          <t># of Subscribers with Arrears</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The number of active subscribers (those receiving and paying for water services) at the beginning of the month.</t>
+          <t>The number of subscribers who have overdue payments for water services.</t>
         </is>
       </c>
     </row>
@@ -651,12 +651,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t># of Active Subscribers at the End of the Month</t>
+          <t># of Subscribers without Water at the End of the Month</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>The number of active subscribers at the end of the month.</t>
+          <t>The number of subscribers who did not receive any water supply by the end of the month.</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t># of Passive Subscribers at the End of the Month</t>
+          <t>Total # of Subscribers</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>The number of subscribers who are registered but are not actively receiving water services at the end of the month.</t>
+          <t>The total count of subscribers, including active, passive, and suspended.</t>
         </is>
       </c>
     </row>
@@ -681,12 +681,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t># of Suspended Subscribers at the End of the Month</t>
+          <t>Residentials</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>The number of subscribers whose services have been temporarily suspended by the end of the month.</t>
+          <t>The number of subscribers classified as residential households.</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t># of Subscribers with Arrears</t>
+          <t>Institutionals</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>The number of subscribers who have overdue payments for water services.</t>
+          <t>The number of subscribers classified as institutions (schools, hospitals, etc.).</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t># of Subscribers without Water at the End of the Month</t>
+          <t>Residential Flat Rate</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>The number of subscribers who did not receive any water supply by the end of the month.</t>
+          <t>The flat rate charged to residential subscribers for water services.</t>
         </is>
       </c>
     </row>
@@ -726,12 +726,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Total # of Subscribers</t>
+          <t>Commercial Flat Rate</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>The total count of subscribers, including active, passive, and suspended.</t>
+          <t>The flat rate charged to commercial subscribers for water services.</t>
         </is>
       </c>
     </row>
@@ -741,12 +741,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Residentials</t>
+          <t>Institutional Flat Rate</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>The number of subscribers classified as residential households.</t>
+          <t>The flat rate charged to institutional subscribers for water services.</t>
         </is>
       </c>
     </row>
@@ -756,12 +756,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Institutionals</t>
+          <t>Commercials</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>The number of subscribers classified as institutions (schools, hospitals, etc.).</t>
+          <t>The number of subscribers classified as commercial businesses.</t>
         </is>
       </c>
     </row>
@@ -771,12 +771,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Residential Flat Rate</t>
+          <t># of Meters Disconnected</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>The flat rate charged to residential subscribers for water services.</t>
+          <t>The number of water meters that have been disconnected either due to non-payment, malfunction, or other reasons.</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Commercial Flat Rate</t>
+          <t># of Meters Reconnected</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>The flat rate charged to commercial subscribers for water services.</t>
+          <t>The number of water meters that have been reconnected after being temporarily disconnected.</t>
         </is>
       </c>
     </row>
@@ -801,12 +801,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Institutional Flat Rate</t>
+          <t># of illegal connections</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>The flat rate charged to institutional subscribers for water services.</t>
+          <t>The number of instances where unauthorized water connections have been detected.</t>
         </is>
       </c>
     </row>
@@ -816,12 +816,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Commercials</t>
+          <t># of illegal connections regularized</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>The number of subscribers classified as commercial businesses.</t>
+          <t>The number of previously unauthorized water intakes that have been regularized (made legal).</t>
         </is>
       </c>
     </row>
@@ -831,12 +831,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t># of Meters Disconnected</t>
+          <t># of Clients with Active Meters</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>The number of water meters that have been disconnected either due to non-payment, malfunction, or other reasons.</t>
+          <t>The number of subscribers who have meters that are currently operating and providing data.</t>
         </is>
       </c>
     </row>
@@ -846,12 +846,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t># of Meters Reconnected</t>
+          <t># of Existing Meters</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>The number of water meters that have been reconnected after being temporarily disconnected.</t>
+          <t>The total number of water meters currently installed within the SAEP's service area.</t>
         </is>
       </c>
     </row>
@@ -861,12 +861,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t># of Illegal Water Intakes</t>
+          <t># of New Installed Meters</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>The number of instances where unauthorized water connections have been detected.</t>
+          <t>The number of new water meters installed during a specific period.</t>
         </is>
       </c>
     </row>
@@ -876,12 +876,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t># of Illegal Water Intakes Regularized</t>
+          <t># of Meters Down</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>The number of previously unauthorized water intakes that have been regularized (made legal).</t>
+          <t>The number of water meters that are malfunctioning or not operational.</t>
         </is>
       </c>
     </row>
@@ -891,12 +891,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t># of Clients with Active Meters</t>
+          <t># of Meters Replaced</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>The number of subscribers who have meters that are currently operating and providing data.</t>
+          <t>The number of old or faulty water meters that have been replaced with new ones.</t>
         </is>
       </c>
     </row>
@@ -906,12 +906,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t># of Existing Meters</t>
+          <t># of Meters Repaired</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>The total number of water meters currently installed within the SAEP's service area.</t>
+          <t>The number of defective water meters that have been repaired and made operational.</t>
         </is>
       </c>
     </row>
@@ -921,12 +921,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t># of New Installed Meters</t>
+          <t># of Clients with Meters</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>The number of new water meters installed during a specific period.</t>
+          <t>The number of subscribers who have water meters installed at their premises.</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t># of Meters Down</t>
+          <t># of Households Served by the SAEP</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>The number of water meters that are malfunctioning or not operational.</t>
+          <t>The total number of households receiving water services from the SAEP.</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t># of Meters Replaced</t>
+          <t># of Individuals Served by the SAEP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>The number of old or faulty water meters that have been replaced with new ones.</t>
+          <t>The total number of individuals benefiting from the water services provided by the SAEP.</t>
         </is>
       </c>
     </row>
@@ -966,12 +966,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t># of Meters Repaired</t>
+          <t># of SAEP Water Production per Household (liters/household/month)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>The number of defective water meters that have been repaired and made operational.</t>
+          <t>The average quantity of water produced by the SAEP per household per month, measured in liters.</t>
         </is>
       </c>
     </row>
@@ -981,12 +981,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t># of Clients with Meters</t>
+          <t>Total Water Produced (m³/month)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>The number of subscribers who have water meters installed at their premises.</t>
+          <t>The total volume of water produced by the SAEP in a month, measured in cubic meters.</t>
         </is>
       </c>
     </row>
@@ -996,12 +996,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t># of Households Served by the SAEP</t>
+          <t>Total Water Distributed (m³/month)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>The total number of households receiving water services from the SAEP.</t>
+          <t>The total volume of water distributed through the SAEP's network in a month, measured in cubic meters.</t>
         </is>
       </c>
     </row>
@@ -1011,12 +1011,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t># of Individuals Served by the SAEP</t>
+          <t>Total Water Consumed (m³/month)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>The total number of individuals benefiting from the water services provided by the SAEP.</t>
+          <t>The total volume of water consumed by end users (households, businesses, institutions) in a month, measured in cubic meters.</t>
         </is>
       </c>
     </row>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t># of SAEP Water Production per Household (liters/household/month)</t>
+          <t>% of Water Loss</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>The average quantity of water produced by the SAEP per household per month, measured in liters.</t>
+          <t>The percentage of water lost (due to leaks, theft, or unaccounted-for usage) compared to the total water produced. Calculated as [(Total Water Produced - Total Water Distributed) / Total Water Produced] * 100.</t>
         </is>
       </c>
     </row>
@@ -1041,12 +1041,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Total Water Produced (m³/month)</t>
+          <t>% of E. Coli Tests Conform</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>The total volume of water produced by the SAEP in a month, measured in cubic meters.</t>
+          <t>The percentage of water quality tests for E. Coli that meet the required safety standards.</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Total Water Distributed (m³/month)</t>
+          <t>% of Residual Chlorine Tests Conforming to Norms</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>The total volume of water distributed through the SAEP’s network in a month, measured in cubic meters.</t>
+          <t>The percentage of water quality tests for residual chlorine that comply with established safety norms.</t>
         </is>
       </c>
     </row>
@@ -1071,12 +1071,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Total Water Consumed (m³/month)</t>
+          <t>Number of Residual Chlorine Tests Conducted</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>The total volume of water consumed by end users (households, businesses, institutions) in a month, measured in cubic meters.</t>
+          <t>The total number of residual chlorine tests conducted to monitor water quality.</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>% of Water Loss</t>
+          <t>Total Revenue (HTG)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>The percentage of water lost (due to leaks, theft, or unaccounted-for usage) compared to the total water produced. Calculated as [(Total Water Produced - Total Water Distributed) / Total Water Produced] * 100.</t>
+          <t>The total income generated by the SAEP from all sources, measured in Haitian Gourdes (HTG).</t>
         </is>
       </c>
     </row>
@@ -1101,12 +1101,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>% of E. Coli Tests Conform</t>
+          <t>Total Expenses (HTG)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>The percentage of water quality tests for E. Coli that meet the required safety standards.</t>
+          <t>The total operating expenses incurred by the SAEP, measured in Haitian Gourdes (HTG).</t>
         </is>
       </c>
     </row>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>% of Residual Chlorine Tests Conforming to Norms</t>
+          <t>Operating Ratio [(Expenses/Revenue) * 100]</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>The percentage of water quality tests for residual chlorine that comply with established safety norms.</t>
+          <t>The operating ratio for a water system is a financial performance metric that indicates how well the system is managing its operating expenses relative to its operating revenues. If the operating ratio is less than 100%: The system is generating more revenue than its operating costs, which indicates financial health and efficiency. If the operating ratio is equal to 100%: The system is breaking even, meaning its revenues are exactly covering its operating expenses. If the operating ratio is greater than 100%: The system is spending more than it earns in revenue, signaling potential financial sustainability issues.</t>
         </is>
       </c>
     </row>
@@ -1131,12 +1131,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Number of Residual Chlorine Tests Conducted</t>
+          <t>Amount Collected from Subscribers (HTG)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>The total number of residual chlorine tests conducted to monitor water quality.</t>
+          <t>The total amount of money collected from subscribers for water services during a specific period, measured in Haitian Gourdes (HTG).</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Total Revenue (HTG)</t>
+          <t>Amount Billed (HTG)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>The total income generated by the SAEP from all sources, measured in Haitian Gourdes (HTG).</t>
+          <t>The total value of bills issued to subscribers for water services during a specific period, measured in Haitian Gourdes (HTG).</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Total Expenses (HTG)</t>
+          <t>Collection Efficiency [(Amount Collected / Amount Billed) * 100]</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>The total operating expenses incurred by the SAEP, measured in Haitian Gourdes (HTG).</t>
+          <t>The efficiency of the SAEP in collecting billed amounts from subscribers. Calculated as (Amount Collected / Amount Billed) * 100.</t>
         </is>
       </c>
     </row>
@@ -1176,12 +1176,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Operating Ratio [(Expenses/Revenue) * 100]</t>
+          <t>Amount Collected Arrears</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>The financial efficiency of the SAEP, calculated as the ratio of total expenses to total revenue, expressed as a percentage.</t>
+          <t>The total amount of overdue payments collected from subscribers during a specific period, measured in Haitian Gourdes (HTG).</t>
         </is>
       </c>
     </row>
@@ -1191,12 +1191,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Amount Collected from Subscribers (HTG)</t>
+          <t>Amount Arrears (Existing at the Start of the Month)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The total amount of money collected from subscribers for water services during a specific period, measured in Haitian Gourdes (HTG).</t>
+          <t>The total amount of overdue payments owed by subscribers at the beginning of the month, measured in Haitian Gourdes (HTG).</t>
         </is>
       </c>
     </row>
@@ -1206,70 +1206,10 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Amount Billed (HTG)</t>
+          <t>Collection Efficiency - Arrears [(Amount Arrears Collected / Amount Arrears at the Start of the Month) * 100]</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
-        <is>
-          <t>The total value of bills issued to subscribers for water services during a specific period, measured in Haitian Gourdes (HTG).</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Collection Efficiency [(Amount Collected / Amount Billed) * 100]</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>The efficiency of the SAEP in collecting billed amounts from subscribers. Calculated as (Amount Collected / Amount Billed) * 100.</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Amount Collected Arrears</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>The total amount of overdue payments collected from subscribers during a specific period, measured in Haitian Gourdes (HTG).</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>54</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Amount Arrears (Existing at the Start of the Month)</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>The total amount of overdue payments owed by subscribers at the beginning of the month, measured in Haitian Gourdes (HTG).</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>55</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Collection Efficiency - Arrears [(Amount Arrears Collected / Amount Arrears at the Start of the Month) * 100]</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
         <is>
           <t>The efficiency of the SAEP in collecting overdue payments from subscribers. Calculated as (Amount Arrears Collected / Amount Arrears at the Start of the Month) * 100.</t>
         </is>

</xml_diff>